<commit_message>
started events, fixed plots in notebook
</commit_message>
<xml_diff>
--- a/Examples/multi_enzyme_model.xlsx
+++ b/Examples/multi_enzyme_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rycar\Documents\GitHub\ODBM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rycar\Documents\GitHub\ODBM\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78471307-2E7F-4662-AA95-74780454FA58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA9B2D7D-69A2-4D6A-8F6E-7F33C1CDE9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{37B5865E-6676-4A0B-967E-9A7116103312}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{37B5865E-6676-4A0B-967E-9A7116103312}"/>
   </bookViews>
   <sheets>
     <sheet name="Species &amp; Base Mechanisms" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="65">
   <si>
     <t>Label</t>
   </si>
@@ -291,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -319,6 +319,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -634,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA16065E-CBBA-49C5-AD56-8DE07546DCC3}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -661,63 +667,64 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>100</v>
-      </c>
+      <c r="C2" s="11">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
       </c>
       <c r="C3">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="C5">
-        <v>1.5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
@@ -728,54 +735,54 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8">
-        <v>0.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
       <c r="C10">
-        <v>0.33</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
         <v>18</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="4" t="s">
-        <v>28</v>
+      <c r="A12" t="s">
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C12">
         <v>0</v>
@@ -783,7 +790,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
@@ -794,7 +801,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
         <v>15</v>
@@ -804,8 +811,8 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="3" t="s">
-        <v>31</v>
+      <c r="A15" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -816,7 +823,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>15</v>
@@ -827,7 +834,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>15</v>
@@ -838,7 +845,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18" t="s">
         <v>15</v>
@@ -849,7 +856,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B19" t="s">
         <v>15</v>
@@ -860,7 +867,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20" t="s">
         <v>15</v>
@@ -871,7 +878,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B21" t="s">
         <v>15</v>
@@ -882,7 +889,7 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
@@ -893,7 +900,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B23" t="s">
         <v>15</v>
@@ -902,8 +909,20 @@
         <v>0</v>
       </c>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B24" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -911,8 +930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542CDD3C-AD6A-49FE-94BE-7648650D73FD}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView zoomScale="101" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E9" sqref="E6:E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
vis update, test folder
</commit_message>
<xml_diff>
--- a/Examples/multi_enzyme_model.xlsx
+++ b/Examples/multi_enzyme_model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rycar\Documents\GitHub\ODBM\Examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Alba\Documents\GitHub\ODBM\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F382496F-AA4B-4CA5-A849-D141BF2D17B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A03FC44-78F7-4AB9-9FA8-04DD7C74DFA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{37B5865E-6676-4A0B-967E-9A7116103312}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{37B5865E-6676-4A0B-967E-9A7116103312}"/>
   </bookViews>
   <sheets>
     <sheet name="Species &amp; Base Mechanisms" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="66">
   <si>
     <t>Label</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Type</t>
   </si>
   <si>
-    <t>CO2</t>
-  </si>
-  <si>
     <t>Metabolite</t>
   </si>
   <si>
@@ -109,9 +106,6 @@
     <t>R2</t>
   </si>
   <si>
-    <t>Pyruvic acid; CO2</t>
-  </si>
-  <si>
     <t>R3</t>
   </si>
   <si>
@@ -235,25 +229,10 @@
     <t>kcat:121600;Km1:3.23;Km2:0.39</t>
   </si>
   <si>
-    <t>R13</t>
-  </si>
-  <si>
-    <t>MA</t>
-  </si>
-  <si>
-    <t>R14</t>
-  </si>
-  <si>
-    <t>R15</t>
-  </si>
-  <si>
-    <t>k:1</t>
-  </si>
-  <si>
-    <t>k:.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
+    <t>HCO3</t>
+  </si>
+  <si>
+    <t>Pyruvic acid;HCO3</t>
   </si>
 </sst>
 </file>
@@ -315,7 +294,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -346,9 +325,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -666,17 +642,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA16065E-CBBA-49C5-AD56-8DE07546DCC3}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A5"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.578125" customWidth="1"/>
-    <col min="4" max="4" width="14.578125" customWidth="1"/>
+    <col min="1" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -684,261 +660,261 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="11">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4">
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
+      <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" t="s">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B15" t="s">
-        <v>14</v>
-      </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B16" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" t="s">
-        <v>14</v>
-      </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A18" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A19" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B19" t="s">
-        <v>14</v>
-      </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A20" s="3" t="s">
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B20" t="s">
-        <v>14</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A21" s="3" t="s">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A22" s="3" t="s">
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" t="s">
-        <v>14</v>
-      </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
-      <c r="A24" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24">
         <v>0</v>
@@ -954,365 +930,332 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542CDD3C-AD6A-49FE-94BE-7648650D73FD}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView zoomScale="101" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="20.578125" customWidth="1"/>
-    <col min="7" max="7" width="40.83984375" customWidth="1"/>
+    <col min="1" max="6" width="20.5703125" customWidth="1"/>
+    <col min="7" max="7" width="40.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="4" t="s">
+      <c r="B2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>21</v>
-      </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="4" t="s">
-        <v>23</v>
-      </c>
       <c r="B3" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E4" s="3"/>
       <c r="F4" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E5" s="3"/>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H6" s="9"/>
       <c r="I6" s="8"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>59</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="8"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="8"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>24</v>
+        <v>65</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="8"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="9"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E12" s="3"/>
       <c r="F12" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="8"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="8"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A14" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G14" s="8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="8" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" s="8" t="s">
-        <v>71</v>
-      </c>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="8"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="4"/>
+      <c r="C15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="8"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="4"/>
+      <c r="C16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>

</xml_diff>

<commit_message>
define concentrations in terms of function/mech
</commit_message>
<xml_diff>
--- a/Examples/multi_enzyme_model.xlsx
+++ b/Examples/multi_enzyme_model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego Alba\Documents\GitHub\ODBM\Examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F25F715C-F7A9-48E3-9D08-0F39BE172CC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E6E52C7-69FB-4CF9-9C71-7E9E46A48C16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{37B5865E-6676-4A0B-967E-9A7116103312}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{37B5865E-6676-4A0B-967E-9A7116103312}"/>
   </bookViews>
   <sheets>
     <sheet name="Species &amp; Base Mechanisms" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="79">
   <si>
     <t>Label</t>
   </si>
@@ -268,79 +268,10 @@
     <t>EXP</t>
   </si>
   <si>
-    <t>R16</t>
-  </si>
-  <si>
-    <t>R17</t>
-  </si>
-  <si>
-    <t>R18</t>
-  </si>
-  <si>
-    <t>R19</t>
-  </si>
-  <si>
-    <t>R20</t>
-  </si>
-  <si>
-    <t>R21</t>
-  </si>
-  <si>
-    <t>R22</t>
-  </si>
-  <si>
-    <t>R23</t>
-  </si>
-  <si>
-    <t>R24</t>
-  </si>
-  <si>
-    <t>R25</t>
-  </si>
-  <si>
-    <t>R26</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
     <t>Cmax:0.05;tau:14400</t>
   </si>
   <si>
-    <t>Sda_Msmeg_DNA</t>
-  </si>
-  <si>
-    <t>Sda_Bsub_DNA</t>
-  </si>
-  <si>
-    <t>Sda_Ecoli_DNA</t>
-  </si>
-  <si>
-    <t>Sda_Lpneu_DNA</t>
-  </si>
-  <si>
-    <t>PCX_Retli_DNA</t>
-  </si>
-  <si>
-    <t>PCX_Scer_DNA</t>
-  </si>
-  <si>
-    <t>PCX_Msmeg_DNA</t>
-  </si>
-  <si>
-    <t>PCX_Gtherm_DNA</t>
-  </si>
-  <si>
-    <t>Mdh_Ecoli_DNA</t>
-  </si>
-  <si>
-    <t>Mdh_Mdom_DNA</t>
-  </si>
-  <si>
-    <t>Mdh_Remer_DNA</t>
-  </si>
-  <si>
-    <t>Mdh_Taes_DNA</t>
+    <t>Conc</t>
   </si>
 </sst>
 </file>
@@ -402,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -433,6 +364,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -748,19 +685,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA16065E-CBBA-49C5-AD56-8DE07546DCC3}">
-  <dimension ref="A1:D36"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25:C36"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25:XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="15.5703125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -771,10 +712,16 @@
         <v>54</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
         <v>3</v>
       </c>
@@ -784,9 +731,9 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>60</v>
       </c>
@@ -797,7 +744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -808,7 +755,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -819,7 +766,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -830,7 +777,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -841,7 +788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -852,7 +799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -863,7 +810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -874,7 +821,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -885,7 +832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -896,271 +843,221 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+    <row r="13" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C13" s="12">
+        <v>0</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C14" s="12">
+        <v>0</v>
+      </c>
+      <c r="D14" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>27</v>
       </c>
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="12">
+        <v>0</v>
+      </c>
+      <c r="D15" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F15" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>13</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C16" s="12">
+        <v>0</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="C17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" s="12">
+        <v>0</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B18" t="s">
         <v>13</v>
       </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" s="12">
+        <v>0</v>
+      </c>
+      <c r="D18" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>31</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="C19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C19" s="12">
+        <v>0</v>
+      </c>
+      <c r="D19" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F19" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B20" t="s">
         <v>13</v>
       </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="12">
+        <v>0</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F20" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>33</v>
       </c>
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="12">
+        <v>0</v>
+      </c>
+      <c r="D21" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>34</v>
       </c>
       <c r="B22" t="s">
         <v>13</v>
       </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="12">
+        <v>0</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>35</v>
       </c>
       <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="C23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="12">
+        <v>0</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>36</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B26" t="s">
-        <v>2</v>
-      </c>
-      <c r="C26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B27" t="s">
-        <v>2</v>
-      </c>
-      <c r="C27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B28" t="s">
-        <v>2</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B29" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B30" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B31" t="s">
-        <v>2</v>
-      </c>
-      <c r="C31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B32" t="s">
-        <v>2</v>
-      </c>
-      <c r="C32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B33" t="s">
-        <v>2</v>
-      </c>
-      <c r="C33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B34" t="s">
-        <v>2</v>
-      </c>
-      <c r="C34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="B35" t="s">
-        <v>2</v>
-      </c>
-      <c r="C35">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B36" t="s">
-        <v>2</v>
-      </c>
-      <c r="C36">
-        <v>0</v>
-      </c>
+      <c r="C24" s="12">
+        <v>0</v>
+      </c>
+      <c r="D24" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="3"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1170,8 +1067,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{542CDD3C-AD6A-49FE-94BE-7648650D73FD}">
   <dimension ref="A1:I42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="101" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31:H42"/>
+    <sheetView zoomScale="101" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1531,208 +1428,88 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A17" s="4"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="8"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G18" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A18" s="4"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="8"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="G19" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A19" s="4"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A20" s="4"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A21" s="4"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A22" s="4"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A23" s="4"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G25" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A25" s="4"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A26" s="4"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A27" s="4"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>89</v>
-      </c>
+      <c r="A28" s="4"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="8"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="F31" s="4"/>

</xml_diff>